<commit_message>
verificar valores de tensao, porque estao muito iguais
</commit_message>
<xml_diff>
--- a/matriz_total.xlsx
+++ b/matriz_total.xlsx
@@ -502,402 +502,402 @@
   <sheetData>
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="n">
-        <v>5</v>
+        <v>2.917480356692093</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>5</v>
+        <v>2.649881837059068</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>6.106611762122174</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>5</v>
+        <v>6.250738792665519</v>
       </c>
       <c r="E1" s="3" t="n">
-        <v>5</v>
+        <v>5.856043773830964</v>
       </c>
       <c r="F1" s="3" t="n">
-        <v>5</v>
+        <v>7.323962829001425</v>
       </c>
       <c r="G1" s="4" t="n">
-        <v>5</v>
+        <v>2.867409350685443</v>
       </c>
       <c r="H1" s="4" t="n">
-        <v>5</v>
+        <v>3.242795707638222</v>
       </c>
       <c r="I1" s="5" t="n">
-        <v>5</v>
+        <v>6.224677088886564</v>
       </c>
       <c r="J1" s="5" t="n">
-        <v>5</v>
+        <v>4.346518932217319</v>
       </c>
       <c r="K1" s="6" t="n">
-        <v>5</v>
+        <v>3.843975048592814</v>
       </c>
       <c r="L1" s="6" t="n">
-        <v>5</v>
+        <v>6.880472713094399</v>
       </c>
       <c r="M1" s="7" t="n">
-        <v>5</v>
+        <v>3.926912292467624</v>
       </c>
       <c r="N1" s="7" t="n">
-        <v>5</v>
+        <v>5.932951174199887</v>
       </c>
       <c r="O1" s="8" t="n">
-        <v>5</v>
+        <v>6.546515913591221</v>
       </c>
       <c r="P1" s="8" t="n">
-        <v>5</v>
+        <v>3.098687113944941</v>
       </c>
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="1" t="n">
-        <v>5</v>
+        <v>4.311654868601988</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>5</v>
+        <v>4.167717804237641</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>5</v>
+        <v>5.710623823757642</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5</v>
+        <v>6.094406305560351</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>5</v>
+        <v>3.912687212042981</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>5</v>
+        <v>7.123437216599187</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>5</v>
+        <v>3.724342390361107</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>5</v>
+        <v>5.986291305383677</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>5</v>
+        <v>6.603634691893245</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>5</v>
+        <v>7.319367752640984</v>
       </c>
       <c r="K2" s="6" t="n">
-        <v>5</v>
+        <v>3.677361685090404</v>
       </c>
       <c r="L2" s="6" t="n">
-        <v>5</v>
+        <v>5.773220447906267</v>
       </c>
       <c r="M2" s="7" t="n">
-        <v>5</v>
+        <v>4.041521261548703</v>
       </c>
       <c r="N2" s="7" t="n">
-        <v>5</v>
+        <v>5.603730946713183</v>
       </c>
       <c r="O2" s="8" t="n">
-        <v>5</v>
+        <v>3.110145845641247</v>
       </c>
       <c r="P2" s="8" t="n">
-        <v>5</v>
+        <v>5.120575436282031</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>5</v>
+        <v>4.119611591735215</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5</v>
+        <v>4.88466187263188</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>5</v>
+        <v>2.836895446529672</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>5</v>
+        <v>3.812872936280541</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>5</v>
+        <v>4.574823203335654</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>5</v>
+        <v>3.029005936731688</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>5</v>
+        <v>7.073765797942427</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>5</v>
+        <v>5.891207778790921</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>5</v>
+        <v>5.6149831180395</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>5</v>
+        <v>6.843504382318262</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>5</v>
+        <v>6.398558338369131</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>5</v>
+        <v>6.843181038857291</v>
       </c>
       <c r="M3" s="8" t="n">
-        <v>5</v>
+        <v>4.405365549842425</v>
       </c>
       <c r="N3" s="8" t="n">
-        <v>5</v>
+        <v>3.237430839985727</v>
       </c>
       <c r="O3" s="5" t="n">
-        <v>5</v>
+        <v>3.889106867124719</v>
       </c>
       <c r="P3" s="5" t="n">
-        <v>5</v>
+        <v>2.671226834697956</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="2" t="n">
-        <v>5</v>
+        <v>6.380770880576456</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5</v>
+        <v>5.541263805585698</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5</v>
+        <v>7.280721063306713</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>5</v>
+        <v>4.529125533362132</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>5</v>
+        <v>4.545536922135314</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>5</v>
+        <v>6.445697513346381</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>5</v>
+        <v>2.873363369870678</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>5</v>
+        <v>4.934525728998567</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>5</v>
+        <v>3.987287662523935</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>5</v>
+        <v>4.513376082293396</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>5</v>
+        <v>5.683755943084341</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>5</v>
+        <v>6.74683351404206</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>5</v>
+        <v>5.223864562892786</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>5</v>
+        <v>4.371675151821418</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>5</v>
+        <v>6.738683713827723</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>5</v>
+        <v>4.504203046849016</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="3" t="n">
-        <v>5</v>
+        <v>2.636288970593771</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>5</v>
+        <v>5.598686549809776</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>5</v>
+        <v>2.74739802392018</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>5</v>
+        <v>2.536365096911963</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>5</v>
+        <v>3.429739756141884</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>5</v>
+        <v>6.466253333489817</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>5</v>
+        <v>6.344867046149227</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>5</v>
+        <v>3.040512771195056</v>
       </c>
       <c r="I5" s="7" t="n">
-        <v>5</v>
+        <v>3.473403369707919</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>5</v>
+        <v>6.649949295352826</v>
       </c>
       <c r="K5" s="8" t="n">
-        <v>5</v>
+        <v>6.758483248944378</v>
       </c>
       <c r="L5" s="8" t="n">
-        <v>5</v>
+        <v>3.616243399157779</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>5</v>
+        <v>5.541543204595959</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>5</v>
+        <v>3.234105784323433</v>
       </c>
       <c r="O5" s="6" t="n">
-        <v>5</v>
+        <v>2.832933872586024</v>
       </c>
       <c r="P5" s="6" t="n">
-        <v>5</v>
+        <v>4.496963876613224</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="3" t="n">
-        <v>5</v>
+        <v>3.06391621393226</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>5</v>
+        <v>5.07119133763026</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>5</v>
+        <v>5.980875592345168</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>5</v>
+        <v>4.986712438241089</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>5</v>
+        <v>3.168238922043614</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>3.052469276988863</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>5</v>
+        <v>7.007887504597622</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>5</v>
+        <v>5.294117944249461</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>5</v>
+        <v>4.44685568629068</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>5</v>
+        <v>5.308785970132625</v>
       </c>
       <c r="K6" s="8" t="n">
-        <v>5</v>
+        <v>4.009546954401521</v>
       </c>
       <c r="L6" s="8" t="n">
-        <v>5</v>
+        <v>5.000604126399675</v>
       </c>
       <c r="M6" s="5" t="n">
-        <v>5</v>
+        <v>3.112390769733419</v>
       </c>
       <c r="N6" s="5" t="n">
-        <v>5</v>
+        <v>6.943033328323473</v>
       </c>
       <c r="O6" s="6" t="n">
-        <v>5</v>
+        <v>4.492547197605632</v>
       </c>
       <c r="P6" s="6" t="n">
-        <v>5</v>
+        <v>6.33356484420021</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="n">
-        <v>5</v>
+        <v>7.052126258872061</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>5</v>
+        <v>3.284047073962878</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>5</v>
+        <v>4.129134392288512</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>5</v>
+        <v>6.948864409065642</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>5</v>
+        <v>3.519547158554324</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>5</v>
+        <v>5.064645641357379</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>5</v>
+        <v>3.013238142272167</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>5</v>
+        <v>6.276379623936763</v>
       </c>
       <c r="I7" s="8" t="n">
-        <v>5</v>
+        <v>7.092778684700678</v>
       </c>
       <c r="J7" s="8" t="n">
-        <v>5</v>
+        <v>3.606190084850887</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>5</v>
+        <v>7.28067303262214</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>5</v>
+        <v>3.968446906587391</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>5</v>
+        <v>6.793344949633989</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>5</v>
+        <v>7.084260598992883</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>5</v>
+        <v>3.790117500957658</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>5</v>
+        <v>7.279343145231868</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="n">
-        <v>5</v>
+        <v>6.957180661685118</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>5</v>
+        <v>6.383950144814563</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>5</v>
+        <v>7.437325332343404</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>5</v>
+        <v>3.685756014176857</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>5</v>
+        <v>3.203837980016258</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>5</v>
+        <v>4.208260308325726</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>5</v>
+        <v>4.05047103332386</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>5</v>
+        <v>3.160385488697595</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>5</v>
+        <v>6.873186153943234</v>
       </c>
       <c r="J8" s="8" t="n">
-        <v>5</v>
+        <v>2.513435225637851</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>5</v>
+        <v>6.365121273357486</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>5</v>
+        <v>5.000669129559636</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>5</v>
+        <v>5.120714812092758</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>5</v>
+        <v>5.628446215810471</v>
       </c>
       <c r="O8" s="7" t="n">
-        <v>5</v>
+        <v>3.382345448911284</v>
       </c>
       <c r="P8" s="7" t="n">
-        <v>5</v>
+        <v>3.927314699748175</v>
       </c>
     </row>
   </sheetData>
@@ -939,402 +939,402 @@
   <sheetData>
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="n">
-        <v>5</v>
+        <v>4.964790473455103</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>5</v>
+        <v>6.854744055578411</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>5.420378417162102</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>5</v>
+        <v>3.267964426388154</v>
       </c>
       <c r="E1" s="3" t="n">
-        <v>5</v>
+        <v>7.431769698280652</v>
       </c>
       <c r="F1" s="3" t="n">
-        <v>5</v>
+        <v>4.456781194463741</v>
       </c>
       <c r="G1" s="4" t="n">
-        <v>5</v>
+        <v>7.233112262445052</v>
       </c>
       <c r="H1" s="4" t="n">
-        <v>5</v>
+        <v>3.298933930069698</v>
       </c>
       <c r="I1" s="5" t="n">
-        <v>5</v>
+        <v>6.229048947468991</v>
       </c>
       <c r="J1" s="5" t="n">
-        <v>5</v>
+        <v>5.077879254855961</v>
       </c>
       <c r="K1" s="6" t="n">
-        <v>5</v>
+        <v>4.929283348126359</v>
       </c>
       <c r="L1" s="6" t="n">
-        <v>5</v>
+        <v>2.598710326022109</v>
       </c>
       <c r="M1" s="7" t="n">
-        <v>5</v>
+        <v>7.424926306139287</v>
       </c>
       <c r="N1" s="7" t="n">
-        <v>5</v>
+        <v>4.569572047202868</v>
       </c>
       <c r="O1" s="8" t="n">
-        <v>5</v>
+        <v>3.229443922253472</v>
       </c>
       <c r="P1" s="8" t="n">
-        <v>5</v>
+        <v>3.684074290872431</v>
       </c>
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="1" t="n">
-        <v>5</v>
+        <v>4.341658724886597</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>5</v>
+        <v>6.580639622671218</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>5</v>
+        <v>2.611320851457358</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5</v>
+        <v>3.70981248833738</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>5</v>
+        <v>5.710797450583516</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>5</v>
+        <v>7.467226478868005</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>5</v>
+        <v>3.286878897096399</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>5</v>
+        <v>5.75697254976418</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>5</v>
+        <v>4.998675578778206</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>5</v>
+        <v>5.393472843949504</v>
       </c>
       <c r="K2" s="6" t="n">
-        <v>5</v>
+        <v>4.503343945362858</v>
       </c>
       <c r="L2" s="6" t="n">
-        <v>5</v>
+        <v>4.298298857382562</v>
       </c>
       <c r="M2" s="7" t="n">
-        <v>5</v>
+        <v>6.138570914881556</v>
       </c>
       <c r="N2" s="7" t="n">
-        <v>5</v>
+        <v>4.421666941830321</v>
       </c>
       <c r="O2" s="8" t="n">
-        <v>5</v>
+        <v>7.117051454264295</v>
       </c>
       <c r="P2" s="8" t="n">
-        <v>5</v>
+        <v>4.793034112653828</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>5</v>
+        <v>5.92444342205707</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5</v>
+        <v>6.817663040821937</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>5</v>
+        <v>4.87031618233153</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>5</v>
+        <v>5.45863805633913</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>5</v>
+        <v>4.750294442286077</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>5</v>
+        <v>7.089139066376624</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>5</v>
+        <v>5.514789894578181</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>5</v>
+        <v>7.183737324545115</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>5</v>
+        <v>5.453620568664565</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>5</v>
+        <v>2.985708399429163</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>5</v>
+        <v>2.595845049952424</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>5</v>
+        <v>4.920599203616503</v>
       </c>
       <c r="M3" s="8" t="n">
-        <v>5</v>
+        <v>3.899256467828241</v>
       </c>
       <c r="N3" s="8" t="n">
-        <v>5</v>
+        <v>3.120772119398563</v>
       </c>
       <c r="O3" s="5" t="n">
-        <v>5</v>
+        <v>6.019756775134294</v>
       </c>
       <c r="P3" s="5" t="n">
-        <v>5</v>
+        <v>4.918427101585201</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="2" t="n">
-        <v>5</v>
+        <v>2.543813809295964</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5</v>
+        <v>2.572741313951961</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5</v>
+        <v>5.105323533923</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>5</v>
+        <v>4.260047150219648</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>5</v>
+        <v>3.332154119761352</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>5</v>
+        <v>2.655292479716778</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>5</v>
+        <v>6.671122720661105</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>5</v>
+        <v>7.238170539920981</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>5</v>
+        <v>3.382171486191473</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>5</v>
+        <v>3.835132866597635</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>5</v>
+        <v>6.013023916864744</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>5</v>
+        <v>4.74652108377568</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>5</v>
+        <v>4.130287714398392</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>5</v>
+        <v>6.713797066992755</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>5</v>
+        <v>5.288009621787601</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>5</v>
+        <v>5.493904826536307</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="3" t="n">
-        <v>5</v>
+        <v>6.116206352127653</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>5</v>
+        <v>6.98780079020751</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>5</v>
+        <v>4.635290358344469</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>5</v>
+        <v>4.380356122900804</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>5</v>
+        <v>6.944428327675362</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>5</v>
+        <v>3.264229437885697</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>5</v>
+        <v>2.987597128814719</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>5</v>
+        <v>3.339594388907137</v>
       </c>
       <c r="I5" s="7" t="n">
-        <v>5</v>
+        <v>3.885258680236048</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>5</v>
+        <v>5.666652534546847</v>
       </c>
       <c r="K5" s="8" t="n">
-        <v>5</v>
+        <v>5.126712671901971</v>
       </c>
       <c r="L5" s="8" t="n">
-        <v>5</v>
+        <v>4.633971884600262</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>5</v>
+        <v>5.125587629162862</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>5</v>
+        <v>7.460417005595388</v>
       </c>
       <c r="O5" s="6" t="n">
-        <v>5</v>
+        <v>7.111355814733916</v>
       </c>
       <c r="P5" s="6" t="n">
-        <v>5</v>
+        <v>4.814619778239935</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="3" t="n">
-        <v>5</v>
+        <v>3.174202384600151</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>5</v>
+        <v>5.934195799826129</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>5</v>
+        <v>7.473477151699514</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>5</v>
+        <v>6.93284285463916</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>5</v>
+        <v>5.88877105273732</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>5.101001600109845</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>5</v>
+        <v>7.493739367783421</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>5</v>
+        <v>6.425914208075585</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>5</v>
+        <v>4.961460560276334</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>5</v>
+        <v>4.718091099496207</v>
       </c>
       <c r="K6" s="8" t="n">
-        <v>5</v>
+        <v>5.444272211145455</v>
       </c>
       <c r="L6" s="8" t="n">
-        <v>5</v>
+        <v>2.990041374347125</v>
       </c>
       <c r="M6" s="5" t="n">
-        <v>5</v>
+        <v>6.053799806930476</v>
       </c>
       <c r="N6" s="5" t="n">
-        <v>5</v>
+        <v>3.941962477976413</v>
       </c>
       <c r="O6" s="6" t="n">
-        <v>5</v>
+        <v>4.85405011549024</v>
       </c>
       <c r="P6" s="6" t="n">
-        <v>5</v>
+        <v>5.798514895298339</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="n">
-        <v>5</v>
+        <v>5.44314273479065</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>5</v>
+        <v>3.094252591759974</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>5</v>
+        <v>3.08193985834221</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>5</v>
+        <v>5.988631445687817</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>5</v>
+        <v>3.323026851388079</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>5</v>
+        <v>5.362783371606263</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>5</v>
+        <v>3.2194394487765</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>5</v>
+        <v>7.106294156135959</v>
       </c>
       <c r="I7" s="8" t="n">
-        <v>5</v>
+        <v>5.931162668793052</v>
       </c>
       <c r="J7" s="8" t="n">
-        <v>5</v>
+        <v>3.206532481525393</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>5</v>
+        <v>3.537040821575921</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>5</v>
+        <v>3.139771409496928</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>5</v>
+        <v>5.590926373020927</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>5</v>
+        <v>3.363507192626937</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>5</v>
+        <v>6.30873764001974</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>5</v>
+        <v>5.990373542162562</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="n">
-        <v>5</v>
+        <v>3.193327767004297</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>5</v>
+        <v>2.501997206603397</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>5</v>
+        <v>5.104675205968983</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>5</v>
+        <v>2.572024439405609</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>5</v>
+        <v>7.102941831960035</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>5</v>
+        <v>5.585789344559561</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>5</v>
+        <v>7.478798635832755</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>5</v>
+        <v>3.297143496238642</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>5</v>
+        <v>3.577228245375053</v>
       </c>
       <c r="J8" s="8" t="n">
-        <v>5</v>
+        <v>5.756210580675798</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>5</v>
+        <v>6.455097162269636</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>5</v>
+        <v>4.969123913650565</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>5</v>
+        <v>4.485418937646051</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>5</v>
+        <v>7.462392777640742</v>
       </c>
       <c r="O8" s="7" t="n">
-        <v>5</v>
+        <v>2.879802545979648</v>
       </c>
       <c r="P8" s="7" t="n">
-        <v>5</v>
+        <v>5.987479255789692</v>
       </c>
     </row>
   </sheetData>
@@ -1376,402 +1376,402 @@
   <sheetData>
     <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="n">
-        <v>5</v>
+        <v>5.663882644882806</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>5</v>
+        <v>4.627138837666146</v>
       </c>
       <c r="C1" s="2" t="n">
-        <v>5</v>
+        <v>2.611041666553048</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>5</v>
+        <v>2.98939990697674</v>
       </c>
       <c r="E1" s="3" t="n">
-        <v>5</v>
+        <v>5.466294290533076</v>
       </c>
       <c r="F1" s="3" t="n">
-        <v>5</v>
+        <v>3.306519787415678</v>
       </c>
       <c r="G1" s="4" t="n">
-        <v>5</v>
+        <v>4.951941014195519</v>
       </c>
       <c r="H1" s="4" t="n">
-        <v>5</v>
+        <v>6.247914205887145</v>
       </c>
       <c r="I1" s="5" t="n">
-        <v>5</v>
+        <v>7.405793700254433</v>
       </c>
       <c r="J1" s="5" t="n">
-        <v>5</v>
+        <v>6.204130350137886</v>
       </c>
       <c r="K1" s="6" t="n">
-        <v>5</v>
+        <v>4.762448287676744</v>
       </c>
       <c r="L1" s="6" t="n">
-        <v>5</v>
+        <v>2.525595398324947</v>
       </c>
       <c r="M1" s="7" t="n">
-        <v>5</v>
+        <v>6.752131494405916</v>
       </c>
       <c r="N1" s="7" t="n">
-        <v>5</v>
+        <v>6.897149634945187</v>
       </c>
       <c r="O1" s="8" t="n">
-        <v>5</v>
+        <v>5.67268796333359</v>
       </c>
       <c r="P1" s="8" t="n">
-        <v>5</v>
+        <v>2.704681019098607</v>
       </c>
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="1" t="n">
-        <v>5</v>
+        <v>3.265234667750346</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>5</v>
+        <v>3.699887542613838</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>5</v>
+        <v>5.451385222251808</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>5</v>
+        <v>4.766212365182103</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>5</v>
+        <v>5.416303064248607</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>5</v>
+        <v>4.727061744548716</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>5</v>
+        <v>6.327750780820618</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>5</v>
+        <v>2.730058680792696</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>5</v>
+        <v>7.331545257432946</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>5</v>
+        <v>6.599470613771898</v>
       </c>
       <c r="K2" s="6" t="n">
-        <v>5</v>
+        <v>3.41419322424695</v>
       </c>
       <c r="L2" s="6" t="n">
-        <v>5</v>
+        <v>6.581159535835759</v>
       </c>
       <c r="M2" s="7" t="n">
-        <v>5</v>
+        <v>4.70901850505839</v>
       </c>
       <c r="N2" s="7" t="n">
-        <v>5</v>
+        <v>2.905358324436643</v>
       </c>
       <c r="O2" s="8" t="n">
-        <v>5</v>
+        <v>3.979569808937082</v>
       </c>
       <c r="P2" s="8" t="n">
-        <v>5</v>
+        <v>6.195421362689571</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="2" t="n">
-        <v>5</v>
+        <v>5.180555464432864</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>5</v>
+        <v>3.992190218676515</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>5</v>
+        <v>6.03710328141669</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>5</v>
+        <v>5.368208201671061</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>5</v>
+        <v>4.1703558079971</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>5</v>
+        <v>7.380450139755832</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>5</v>
+        <v>3.777061050971595</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>5</v>
+        <v>4.448000818416403</v>
       </c>
       <c r="I3" s="6" t="n">
-        <v>5</v>
+        <v>4.354404065319757</v>
       </c>
       <c r="J3" s="6" t="n">
-        <v>5</v>
+        <v>5.258346741937745</v>
       </c>
       <c r="K3" s="7" t="n">
-        <v>5</v>
+        <v>6.85045885474578</v>
       </c>
       <c r="L3" s="7" t="n">
-        <v>5</v>
+        <v>3.618235796850936</v>
       </c>
       <c r="M3" s="8" t="n">
-        <v>5</v>
+        <v>4.072336232174899</v>
       </c>
       <c r="N3" s="8" t="n">
-        <v>5</v>
+        <v>5.908252239502215</v>
       </c>
       <c r="O3" s="5" t="n">
-        <v>5</v>
+        <v>5.08437621355378</v>
       </c>
       <c r="P3" s="5" t="n">
-        <v>5</v>
+        <v>6.929401219555384</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="2" t="n">
-        <v>5</v>
+        <v>3.75550617577747</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>5</v>
+        <v>6.412866694353463</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5</v>
+        <v>4.883125743038078</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>5</v>
+        <v>6.669679651889524</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>5</v>
+        <v>5.974925477984324</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>5</v>
+        <v>4.398340397175444</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>5</v>
+        <v>7.294046416968216</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>5</v>
+        <v>4.52666372145138</v>
       </c>
       <c r="I4" s="6" t="n">
-        <v>5</v>
+        <v>4.643348420321636</v>
       </c>
       <c r="J4" s="6" t="n">
-        <v>5</v>
+        <v>4.374133795809213</v>
       </c>
       <c r="K4" s="7" t="n">
-        <v>5</v>
+        <v>6.894349155754107</v>
       </c>
       <c r="L4" s="7" t="n">
-        <v>5</v>
+        <v>3.956465566344767</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v>5</v>
+        <v>6.4448801526423</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>5</v>
+        <v>3.295848718961496</v>
       </c>
       <c r="O4" s="5" t="n">
-        <v>5</v>
+        <v>2.715597161235285</v>
       </c>
       <c r="P4" s="5" t="n">
-        <v>5</v>
+        <v>6.545675025660135</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="3" t="n">
-        <v>5</v>
+        <v>4.88489974278814</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>5</v>
+        <v>3.839014243634673</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>5</v>
+        <v>6.921072525426863</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>5</v>
+        <v>6.207841074535065</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>5</v>
+        <v>2.567127090452251</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>5</v>
+        <v>4.581952984092882</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>5</v>
+        <v>6.245186095260001</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>5</v>
+        <v>6.674404771310092</v>
       </c>
       <c r="I5" s="7" t="n">
-        <v>5</v>
+        <v>6.459690260577455</v>
       </c>
       <c r="J5" s="7" t="n">
-        <v>5</v>
+        <v>3.322222607601566</v>
       </c>
       <c r="K5" s="8" t="n">
-        <v>5</v>
+        <v>4.021717092671088</v>
       </c>
       <c r="L5" s="8" t="n">
-        <v>5</v>
+        <v>3.827203681916637</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>5</v>
+        <v>4.414908306516551</v>
       </c>
       <c r="N5" s="5" t="n">
-        <v>5</v>
+        <v>6.115628733102332</v>
       </c>
       <c r="O5" s="6" t="n">
-        <v>5</v>
+        <v>2.525310784610165</v>
       </c>
       <c r="P5" s="6" t="n">
-        <v>5</v>
+        <v>5.566171545577139</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="3" t="n">
-        <v>5</v>
+        <v>4.98476796581518</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>5</v>
+        <v>6.44231779874893</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>5</v>
+        <v>3.0664518115357</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>5</v>
+        <v>7.271233302432325</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>5</v>
+        <v>5.296217457959937</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>5</v>
+        <v>3.330486162862079</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>5</v>
+        <v>5.224579463868864</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>5</v>
+        <v>6.673273578525684</v>
       </c>
       <c r="I6" s="7" t="n">
-        <v>5</v>
+        <v>6.188079428475676</v>
       </c>
       <c r="J6" s="7" t="n">
-        <v>5</v>
+        <v>3.612582557473178</v>
       </c>
       <c r="K6" s="8" t="n">
-        <v>5</v>
+        <v>4.754470580757824</v>
       </c>
       <c r="L6" s="8" t="n">
-        <v>5</v>
+        <v>3.212275701308926</v>
       </c>
       <c r="M6" s="5" t="n">
-        <v>5</v>
+        <v>3.732957483678242</v>
       </c>
       <c r="N6" s="5" t="n">
-        <v>5</v>
+        <v>4.279948307507771</v>
       </c>
       <c r="O6" s="6" t="n">
-        <v>5</v>
+        <v>3.32656858150604</v>
       </c>
       <c r="P6" s="6" t="n">
-        <v>5</v>
+        <v>6.545541138885403</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="n">
-        <v>5</v>
+        <v>4.983154431771559</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>5</v>
+        <v>4.65550286030708</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>5</v>
+        <v>4.663708079881786</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>5</v>
+        <v>4.399863217133128</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>5</v>
+        <v>6.220639805868835</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>5</v>
+        <v>6.398368663760898</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>5</v>
+        <v>2.880848452148995</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>5</v>
+        <v>6.625827617460152</v>
       </c>
       <c r="I7" s="8" t="n">
-        <v>5</v>
+        <v>7.032966287700855</v>
       </c>
       <c r="J7" s="8" t="n">
-        <v>5</v>
+        <v>2.560963902657472</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>5</v>
+        <v>6.305449968565085</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>5</v>
+        <v>7.243358118751642</v>
       </c>
       <c r="M7" s="6" t="n">
-        <v>5</v>
+        <v>4.838290035118964</v>
       </c>
       <c r="N7" s="6" t="n">
-        <v>5</v>
+        <v>6.958192647732155</v>
       </c>
       <c r="O7" s="7" t="n">
-        <v>5</v>
+        <v>6.113390186562393</v>
       </c>
       <c r="P7" s="7" t="n">
-        <v>5</v>
+        <v>6.293702924716817</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="n">
-        <v>5</v>
+        <v>4.799861810386895</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>5</v>
+        <v>5.07491242571419</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>5</v>
+        <v>5.050327574187947</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>5</v>
+        <v>6.328241100385412</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>5</v>
+        <v>2.97216761641844</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>5</v>
+        <v>7.126807920189461</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>5</v>
+        <v>5.743181114220228</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>5</v>
+        <v>6.603728908418304</v>
       </c>
       <c r="I8" s="8" t="n">
-        <v>5</v>
+        <v>7.488399529371533</v>
       </c>
       <c r="J8" s="8" t="n">
-        <v>5</v>
+        <v>6.029301060448958</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>5</v>
+        <v>3.063610574934054</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>5</v>
+        <v>3.073871923769225</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>5</v>
+        <v>3.97593586828195</v>
       </c>
       <c r="N8" s="6" t="n">
-        <v>5</v>
+        <v>7.247392059599451</v>
       </c>
       <c r="O8" s="7" t="n">
-        <v>5</v>
+        <v>4.230489322772445</v>
       </c>
       <c r="P8" s="7" t="n">
-        <v>5</v>
+        <v>6.142470580260663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>